<commit_message>
Decode API results: reading JSON in PHP
</commit_message>
<xml_diff>
--- a/me/1.api-basics.xlsx
+++ b/me/1.api-basics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4ED7A49-A9CD-448F-8151-7ECE2034C8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7DB2D8-0199-41EA-8B02-7F348776CF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Make an API call" sheetId="1" r:id="rId1"/>
+    <sheet name="Decode API results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>RANDOM USER GENERATOR</t>
   </si>
@@ -98,6 +99,52 @@
       </rPr>
       <t>("https://randomuser.me/api");</t>
     </r>
+  </si>
+  <si>
+    <t>→</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>2.decode-api-results</t>
+  </si>
+  <si>
+    <t>rest-api-php\1.api-basics\2.decode-api-results\index.php</t>
+  </si>
+  <si>
+    <t>$response = file_get_contents("https://randomuser.me/api");</t>
+  </si>
+  <si>
+    <t>echo $data["results"][0]["name"]["first"], "\n";</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$data = json_decode($response, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>Truyền thêm tham số thứ 2 là true để giá trị trả về ở dạng mảng</t>
   </si>
 </sst>
 </file>
@@ -306,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -328,6 +375,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,6 +579,161 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CF656AC-1E18-0933-CFD2-A0FEE6FE9B5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="847725" y="17154525"/>
+          <a:ext cx="371475" cy="1247775"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>237412</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123631</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96F27F4F-9A61-7DDB-D9D0-C95B1175C7C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="4286250"/>
+          <a:ext cx="5704762" cy="1552381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFAE26A9-8941-51C7-1D82-CFF7C44195E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="828675" y="3581400"/>
+          <a:ext cx="66675" cy="1390650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -800,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:U93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="J81" sqref="J81"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="K87" sqref="K87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2443,7 +2647,7 @@
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" s="8"/>
       <c r="C81" s="6"/>
-      <c r="D81" s="6" t="s">
+      <c r="D81" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E81" s="7"/>
@@ -2452,8 +2656,14 @@
       <c r="B82" s="9"/>
       <c r="C82" s="10"/>
       <c r="D82" s="10"/>
-      <c r="E82" s="11" t="s">
+      <c r="E82" s="21" t="s">
         <v>9</v>
+      </c>
+      <c r="F82" t="s">
+        <v>17</v>
+      </c>
+      <c r="G82" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2517,4 +2727,154 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0BC13D-53F9-4FEA-92D9-E1038EE0F50C}">
+  <dimension ref="A4:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Use API data in a web application
</commit_message>
<xml_diff>
--- a/me/1.api-basics.xlsx
+++ b/me/1.api-basics.xlsx
@@ -8,25 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7DB2D8-0199-41EA-8B02-7F348776CF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0684C1BD-2BA4-41CF-9C29-A81A71484CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Make an API call" sheetId="1" r:id="rId1"/>
     <sheet name="Decode API results" sheetId="2" r:id="rId2"/>
+    <sheet name="Use API data in a web app" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>RANDOM USER GENERATOR</t>
   </si>
@@ -145,6 +154,102 @@
   </si>
   <si>
     <t>Truyền thêm tham số thứ 2 là true để giá trị trả về ở dạng mảng</t>
+  </si>
+  <si>
+    <t>Predict the age of a name</t>
+  </si>
+  <si>
+    <t>https://agify.io/</t>
+  </si>
+  <si>
+    <t>https://api.agify.io/?name=michael</t>
+  </si>
+  <si>
+    <t>3.use-api-data-in-a-web-application</t>
+  </si>
+  <si>
+    <t>Dùng api agify để dự đoán tuổi dựa vào tên</t>
+  </si>
+  <si>
+    <t>rest-api-php\1.api-basics\3.use-api-data-in-a-web-application\index.php</t>
+  </si>
+  <si>
+    <t>if (!empty($_GET["name"])) {</t>
+  </si>
+  <si>
+    <t>    $response = file_get_contents("https://api.agify.io?name={$_GET['name']}");</t>
+  </si>
+  <si>
+    <t>    $data = json_decode($response, true);</t>
+  </si>
+  <si>
+    <t>    $age = $data["age"];</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>?&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!DOCTYPE html&gt;</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;</t>
+  </si>
+  <si>
+    <t>&lt;head&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;title&gt;Example&lt;/title&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/head&gt;</t>
+  </si>
+  <si>
+    <t>&lt;body&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;?php if (isset($age)) : ?&gt;</t>
+  </si>
+  <si>
+    <t>        Age: &lt;?= $age ?&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;?php endif; ?&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;form&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;label for="name"&gt;Name&lt;/label&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;input name="name" id="name"&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;button&gt;Guess age&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;/form&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/body&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>Nhập tên</t>
+  </si>
+  <si>
+    <t>Lấy tuổi từ kết quả api agify trả về</t>
+  </si>
+  <si>
+    <t>Nhập tên là Dave để tìm kiếm</t>
+  </si>
+  <si>
+    <t>Có tuổi từ api trả về thì in ra màn hình</t>
   </si>
 </sst>
 </file>
@@ -353,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -377,6 +482,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,6 +849,565 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>42235</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8175B5A0-FF2E-63C4-8944-08A1530E7C6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="1457326"/>
+          <a:ext cx="11172825" cy="4880934"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C432546A-DE2C-FDF3-EB84-3CDEBE7CF4CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1343025" y="1343025"/>
+          <a:ext cx="4371975" cy="3705225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>220350</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5468E710-B36F-AF9A-56AB-52713439EFD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="771524" y="6762750"/>
+          <a:ext cx="11021701" cy="1866900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{562A8769-DC2D-A996-C3E9-15BC745763D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3648075" y="5238750"/>
+          <a:ext cx="2257425" cy="1619250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C45533A4-E8FF-B2AE-4F38-4331143DFA31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1781175" y="11811000"/>
+          <a:ext cx="762000" cy="5229225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF5F8CB0-12FE-F089-011A-A589C8AD2AB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="11791950"/>
+          <a:ext cx="1857375" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E55B368-33A4-5735-5530-63E915120AD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="12915900"/>
+          <a:ext cx="876300" cy="2428875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>399101</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>85557</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A55FE03-F25F-D3E2-5F3B-79D2F03B85CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="19335750"/>
+          <a:ext cx="7590476" cy="1342857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>174335</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1670AFA9-0858-F4FB-C473-C240CED9FCB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="21402674"/>
+          <a:ext cx="7391400" cy="1650711"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Arrow: Down 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28A5375F-1576-6AB4-A595-58BD6E2FC0AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3181350" y="20916900"/>
+          <a:ext cx="209550" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C61C8B-390F-0B65-CA14-EC241D0C721D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1266825" y="12954000"/>
+          <a:ext cx="4248150" cy="9258300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1004,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:U93"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="K87" sqref="K87"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2733,8 +3402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0BC13D-53F9-4FEA-92D9-E1038EE0F50C}">
   <dimension ref="A4:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,4 +3546,1842 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66420E95-12AE-4222-BAB7-D3D0AF738400}">
+  <dimension ref="A2:T122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="L73" sqref="L73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="14"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="16"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="16"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="16"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="16"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="16"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="16"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="16"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="16"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="16"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="16"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="16"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="16"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="16"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="16"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="16"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="16"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="16"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="16"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="16"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="16"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="16"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="16"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="16"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="16"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="16"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="16"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="16"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="16"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="15"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6"/>
+      <c r="T34" s="16"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="16"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="16"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="16"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+      <c r="T38" s="16"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6"/>
+      <c r="T39" s="16"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="15"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+      <c r="T40" s="16"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="16"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="6"/>
+      <c r="T42" s="16"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="6"/>
+      <c r="T43" s="16"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="15"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="6"/>
+      <c r="T44" s="16"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="15"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="16"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="15"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="6"/>
+      <c r="T46" s="16"/>
+    </row>
+    <row r="47" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="17"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
+      <c r="T47" s="19"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="8"/>
+      <c r="C52" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="7"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="8"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="8"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="8"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="7"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="9"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="10"/>
+      <c r="G56" s="11"/>
+      <c r="H56" t="s">
+        <v>17</v>
+      </c>
+      <c r="I56" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="8"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="7"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="7"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="8"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="7"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="7"/>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B65" s="8"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="7"/>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B66" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="7"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" s="8"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="7"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="7"/>
+      <c r="J68" t="s">
+        <v>17</v>
+      </c>
+      <c r="K68" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="7"/>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70" s="8"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="7"/>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="7"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B72" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="7"/>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B73" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="7"/>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B74" s="8"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="7"/>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B75" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="7"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B76" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="7"/>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B77" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="7"/>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B78" s="8"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="7"/>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B79" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="7"/>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B80" s="8"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="7"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B81" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="7"/>
+      <c r="J81" t="str">
+        <f>$J$68</f>
+        <v>→</v>
+      </c>
+      <c r="K81" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B82" s="8"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="7"/>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B83" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="7"/>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B84" s="8"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="7"/>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B85" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="7"/>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B86" s="8"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="7"/>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B87" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="7"/>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B88" s="8"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="7"/>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B89" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="7"/>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B90" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="7"/>
+      <c r="J90" t="s">
+        <v>17</v>
+      </c>
+      <c r="K90" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B91" s="8"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="7"/>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B92" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="7"/>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B93" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="7"/>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B94" s="8"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="7"/>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B95" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="7"/>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B96" s="8"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="7"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B97" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="11"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B101" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="3"/>
+      <c r="M101" s="3"/>
+      <c r="N101" s="4"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B102" s="8"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6"/>
+      <c r="M102" s="6"/>
+      <c r="N102" s="7"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B103" s="8"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="6"/>
+      <c r="M103" s="6"/>
+      <c r="N103" s="7"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B104" s="8"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6"/>
+      <c r="K104" s="6"/>
+      <c r="L104" s="6"/>
+      <c r="M104" s="6"/>
+      <c r="N104" s="7"/>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B105" s="8"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="6"/>
+      <c r="M105" s="6"/>
+      <c r="N105" s="7"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B106" s="8"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="6"/>
+      <c r="M106" s="6"/>
+      <c r="N106" s="7"/>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B107" s="8"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
+      <c r="K107" s="6"/>
+      <c r="L107" s="6"/>
+      <c r="M107" s="6"/>
+      <c r="N107" s="7"/>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B108" s="8"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="6"/>
+      <c r="M108" s="6"/>
+      <c r="N108" s="7"/>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B109" s="8"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+      <c r="J109" s="6"/>
+      <c r="K109" s="6"/>
+      <c r="L109" s="6"/>
+      <c r="M109" s="6"/>
+      <c r="N109" s="7"/>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B110" s="8"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="6"/>
+      <c r="M110" s="6"/>
+      <c r="N110" s="7"/>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B111" s="8"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="6"/>
+      <c r="K111" s="6"/>
+      <c r="L111" s="6"/>
+      <c r="M111" s="6"/>
+      <c r="N111" s="7"/>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B112" s="8"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="6"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="6"/>
+      <c r="J112" s="6"/>
+      <c r="K112" s="6"/>
+      <c r="L112" s="6"/>
+      <c r="M112" s="6"/>
+      <c r="N112" s="7"/>
+    </row>
+    <row r="113" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B113" s="8"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
+      <c r="K113" s="6"/>
+      <c r="L113" s="6"/>
+      <c r="M113" s="6"/>
+      <c r="N113" s="7"/>
+    </row>
+    <row r="114" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B114" s="8"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="6"/>
+      <c r="K114" s="6"/>
+      <c r="L114" s="6"/>
+      <c r="M114" s="6"/>
+      <c r="N114" s="7"/>
+    </row>
+    <row r="115" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B115" s="8"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="6"/>
+      <c r="K115" s="6"/>
+      <c r="L115" s="6"/>
+      <c r="M115" s="6"/>
+      <c r="N115" s="7"/>
+    </row>
+    <row r="116" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B116" s="8"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+      <c r="J116" s="6"/>
+      <c r="K116" s="6"/>
+      <c r="L116" s="6"/>
+      <c r="M116" s="6"/>
+      <c r="N116" s="7"/>
+    </row>
+    <row r="117" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B117" s="8"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="6"/>
+      <c r="J117" s="6"/>
+      <c r="K117" s="6"/>
+      <c r="L117" s="6"/>
+      <c r="M117" s="6"/>
+      <c r="N117" s="7"/>
+    </row>
+    <row r="118" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B118" s="8"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="6"/>
+      <c r="J118" s="6"/>
+      <c r="K118" s="6"/>
+      <c r="L118" s="6"/>
+      <c r="M118" s="6"/>
+      <c r="N118" s="7"/>
+    </row>
+    <row r="119" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B119" s="8"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="6"/>
+      <c r="I119" s="6"/>
+      <c r="J119" s="6"/>
+      <c r="K119" s="6"/>
+      <c r="L119" s="6"/>
+      <c r="M119" s="6"/>
+      <c r="N119" s="7"/>
+    </row>
+    <row r="120" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B120" s="8"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6"/>
+      <c r="I120" s="6"/>
+      <c r="J120" s="6"/>
+      <c r="K120" s="6"/>
+      <c r="L120" s="6"/>
+      <c r="M120" s="6"/>
+      <c r="N120" s="7"/>
+    </row>
+    <row r="121" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B121" s="8"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+      <c r="H121" s="6"/>
+      <c r="I121" s="6"/>
+      <c r="J121" s="6"/>
+      <c r="K121" s="6"/>
+      <c r="L121" s="6"/>
+      <c r="M121" s="6"/>
+      <c r="N121" s="7"/>
+    </row>
+    <row r="122" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B122" s="9"/>
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="10"/>
+      <c r="G122" s="10"/>
+      <c r="H122" s="10"/>
+      <c r="I122" s="10"/>
+      <c r="J122" s="10"/>
+      <c r="K122" s="10"/>
+      <c r="L122" s="10"/>
+      <c r="M122" s="10"/>
+      <c r="N122" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Use cURL instead of file_get_contents to make an API request
</commit_message>
<xml_diff>
--- a/me/1.api-basics.xlsx
+++ b/me/1.api-basics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0684C1BD-2BA4-41CF-9C29-A81A71484CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3182EF4C-24FE-44EB-80B0-35C3CD17113E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>RANDOM USER GENERATOR</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>Có tuổi từ api trả về thì in ra màn hình</t>
+  </si>
+  <si>
+    <t>Make an API call: access an API from PHP</t>
+  </si>
+  <si>
+    <t>Decode API results: reading JSON in PHP</t>
+  </si>
+  <si>
+    <t>Use API data in a web application</t>
   </si>
 </sst>
 </file>
@@ -510,13 +519,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>81922</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -540,7 +549,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="761999" y="1247775"/>
+          <a:off x="761999" y="1447800"/>
           <a:ext cx="11191875" cy="5501647"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -554,13 +563,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>423738</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -584,7 +593,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="723900" y="7496175"/>
+          <a:off x="723900" y="7696200"/>
           <a:ext cx="11348913" cy="5724525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -598,13 +607,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -620,7 +629,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="704850" y="7400925"/>
+          <a:off x="704850" y="7591425"/>
           <a:ext cx="1981200" cy="9239250"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -651,13 +660,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>104</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>9748</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -681,7 +690,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="638175" y="17821275"/>
+          <a:off x="638175" y="18011775"/>
           <a:ext cx="11430000" cy="2019523"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -695,13 +704,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -717,7 +726,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="847725" y="17154525"/>
+          <a:off x="847725" y="17345025"/>
           <a:ext cx="371475" cy="1247775"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -855,13 +864,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>42235</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -885,7 +894,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="695325" y="1457326"/>
+          <a:off x="695325" y="1647826"/>
           <a:ext cx="11172825" cy="4880934"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -899,13 +908,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -921,7 +930,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1343025" y="1343025"/>
+          <a:off x="1343025" y="1533525"/>
           <a:ext cx="4371975" cy="3705225"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -952,13 +961,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>161924</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>220350</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -982,7 +991,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="771524" y="6762750"/>
+          <a:off x="771524" y="6953250"/>
           <a:ext cx="11021701" cy="1866900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -996,13 +1005,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1018,7 +1027,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3648075" y="5238750"/>
+          <a:off x="3648075" y="5429250"/>
           <a:ext cx="2257425" cy="1619250"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1049,13 +1058,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1071,7 +1080,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="1781175" y="11811000"/>
+          <a:off x="1781175" y="12001500"/>
           <a:ext cx="762000" cy="5229225"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1102,13 +1111,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1124,7 +1133,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2047875" y="11791950"/>
+          <a:off x="2047875" y="11982450"/>
           <a:ext cx="1857375" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1155,13 +1164,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1177,7 +1186,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="838200" y="12915900"/>
+          <a:off x="838200" y="13106400"/>
           <a:ext cx="876300" cy="2428875"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1208,13 +1217,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>102</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>399101</xdr:colOff>
-      <xdr:row>108</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>85557</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1238,7 +1247,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="723900" y="19335750"/>
+          <a:off x="723900" y="19526250"/>
           <a:ext cx="7590476" cy="1342857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1252,13 +1261,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>174335</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1282,7 +1291,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="733425" y="21402674"/>
+          <a:off x="733425" y="21593174"/>
           <a:ext cx="7391400" cy="1650711"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1296,13 +1305,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1318,7 +1327,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3181350" y="20916900"/>
+          <a:off x="3181350" y="21107400"/>
           <a:ext cx="209550" cy="400050"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
@@ -1356,13 +1365,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>116</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1378,7 +1387,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1266825" y="12954000"/>
+          <a:off x="1266825" y="13144500"/>
           <a:ext cx="4248150" cy="9258300"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1671,10 +1680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:U93"/>
+  <dimension ref="A2:U94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,87 +1691,69 @@
     <col min="5" max="5" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="14"/>
-    </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="16"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="14"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
-      <c r="B6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="7"/>
+      <c r="B6" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="4"/>
       <c r="U6" s="16"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="8"/>
+      <c r="B7" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -2429,103 +2420,103 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
-      <c r="T36" s="11"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="7"/>
       <c r="U36" s="16"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
-      <c r="T37" s="6"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="11"/>
       <c r="U37" s="16"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
-      <c r="B38" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
-      <c r="T38" s="4"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+      <c r="T38" s="6"/>
       <c r="U38" s="16"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
-      <c r="B39" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="6"/>
-      <c r="T39" s="7"/>
+      <c r="B39" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="4"/>
       <c r="U39" s="16"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
-      <c r="B40" s="8"/>
+      <c r="B40" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -3238,130 +3229,143 @@
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="15"/>
-      <c r="B71" s="9"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
-      <c r="G71" s="10"/>
-      <c r="H71" s="10"/>
-      <c r="I71" s="10"/>
-      <c r="J71" s="10"/>
-      <c r="K71" s="10"/>
-      <c r="L71" s="10"/>
-      <c r="M71" s="10"/>
-      <c r="N71" s="10"/>
-      <c r="O71" s="10"/>
-      <c r="P71" s="10"/>
-      <c r="Q71" s="10"/>
-      <c r="R71" s="10"/>
-      <c r="S71" s="10"/>
-      <c r="T71" s="11"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="6"/>
+      <c r="P71" s="6"/>
+      <c r="Q71" s="6"/>
+      <c r="R71" s="6"/>
+      <c r="S71" s="6"/>
+      <c r="T71" s="7"/>
       <c r="U71" s="16"/>
     </row>
-    <row r="72" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="17"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
-      <c r="J72" s="18"/>
-      <c r="K72" s="18"/>
-      <c r="L72" s="18"/>
-      <c r="M72" s="18"/>
-      <c r="N72" s="18"/>
-      <c r="O72" s="18"/>
-      <c r="P72" s="18"/>
-      <c r="Q72" s="18"/>
-      <c r="R72" s="18"/>
-      <c r="S72" s="18"/>
-      <c r="T72" s="18"/>
-      <c r="U72" s="19"/>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A72" s="15"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="10"/>
+      <c r="L72" s="10"/>
+      <c r="M72" s="10"/>
+      <c r="N72" s="10"/>
+      <c r="O72" s="10"/>
+      <c r="P72" s="10"/>
+      <c r="Q72" s="10"/>
+      <c r="R72" s="10"/>
+      <c r="S72" s="10"/>
+      <c r="T72" s="11"/>
+      <c r="U72" s="16"/>
+    </row>
+    <row r="73" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="17"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+      <c r="J73" s="18"/>
+      <c r="K73" s="18"/>
+      <c r="L73" s="18"/>
+      <c r="M73" s="18"/>
+      <c r="N73" s="18"/>
+      <c r="O73" s="18"/>
+      <c r="P73" s="18"/>
+      <c r="Q73" s="18"/>
+      <c r="R73" s="18"/>
+      <c r="S73" s="18"/>
+      <c r="T73" s="18"/>
+      <c r="U73" s="19"/>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B79" s="2" t="s">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="4"/>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B80" s="8"/>
-      <c r="C80" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D80" s="6"/>
-      <c r="E80" s="7"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="4"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B81" s="8"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="22" t="s">
+      <c r="C81" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="6"/>
+      <c r="E81" s="7"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="8"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E81" s="7"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="9"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="21" t="s">
+      <c r="E82" s="7"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="9"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F83" t="s">
         <v>17</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G83" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="2" t="s">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="4"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="8"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="6"/>
-      <c r="G87" s="7"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="4"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B88" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="B88" s="8"/>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
       <c r="E88" s="6"/>
@@ -3369,7 +3373,9 @@
       <c r="G88" s="7"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="8"/>
+      <c r="B89" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
@@ -3377,17 +3383,25 @@
       <c r="G89" s="7"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B90" s="9" t="s">
+      <c r="B90" s="8"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="7"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C90" s="10"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="11"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="11"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3400,10 +3414,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0BC13D-53F9-4FEA-92D9-E1038EE0F50C}">
-  <dimension ref="A4:I22"/>
+  <dimension ref="A2:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3411,6 +3425,11 @@
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
@@ -3550,10 +3569,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66420E95-12AE-4222-BAB7-D3D0AF738400}">
-  <dimension ref="A2:T122"/>
+  <dimension ref="A2:T123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="L73" sqref="L73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" activeCellId="1" sqref="B2 I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3563,65 +3582,46 @@
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="14"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="16"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="14"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
-      <c r="B7" s="24" t="s">
-        <v>27</v>
-      </c>
+      <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -3643,7 +3643,9 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
-      <c r="B8" s="6"/>
+      <c r="B8" s="24" t="s">
+        <v>27</v>
+      </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -4499,59 +4501,71 @@
       <c r="S46" s="6"/>
       <c r="T46" s="16"/>
     </row>
-    <row r="47" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="17"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="19"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="15"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="6"/>
+      <c r="T47" s="16"/>
+    </row>
+    <row r="48" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="17"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
+      <c r="T48" s="19"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="2" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="4"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="8"/>
-      <c r="C52" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="7"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="4"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="C53" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
       <c r="G53" s="7"/>
@@ -4559,8 +4573,8 @@
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B54" s="8"/>
       <c r="C54" s="6"/>
-      <c r="D54" s="26" t="s">
-        <v>19</v>
+      <c r="D54" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -4569,60 +4583,58 @@
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B55" s="8"/>
       <c r="C55" s="6"/>
-      <c r="D55" s="22" t="s">
-        <v>28</v>
+      <c r="D55" s="26" t="s">
+        <v>19</v>
       </c>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
       <c r="G55" s="7"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="9"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="27" t="s">
+      <c r="B56" s="8"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="7"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="9"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F56" s="10"/>
-      <c r="G56" s="11"/>
-      <c r="H56" t="s">
+      <c r="F57" s="10"/>
+      <c r="G57" s="11"/>
+      <c r="H57" t="s">
         <v>17</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I57" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="2" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="4"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="8"/>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="7"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="4"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="B62" s="8"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
@@ -4632,7 +4644,9 @@
       <c r="I62" s="7"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="8"/>
+      <c r="B63" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
@@ -4642,9 +4656,7 @@
       <c r="I63" s="7"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="B64" s="8"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
@@ -4654,7 +4666,9 @@
       <c r="I64" s="7"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B65" s="8"/>
+      <c r="B65" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
@@ -4664,9 +4678,7 @@
       <c r="I65" s="7"/>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B66" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="B66" s="8"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
@@ -4676,7 +4688,9 @@
       <c r="I66" s="7"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B67" s="8"/>
+      <c r="B67" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
@@ -4686,9 +4700,7 @@
       <c r="I67" s="7"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B68" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="B68" s="8"/>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
@@ -4696,16 +4708,10 @@
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
       <c r="I68" s="7"/>
-      <c r="J68" t="s">
-        <v>17</v>
-      </c>
-      <c r="K68" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
@@ -4714,9 +4720,17 @@
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
       <c r="I69" s="7"/>
+      <c r="J69" t="s">
+        <v>17</v>
+      </c>
+      <c r="K69" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B70" s="8"/>
+      <c r="B70" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
@@ -4726,9 +4740,7 @@
       <c r="I70" s="7"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B71" s="8" t="s">
-        <v>36</v>
-      </c>
+      <c r="B71" s="8"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
@@ -4739,7 +4751,7 @@
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
@@ -4751,7 +4763,7 @@
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
@@ -4762,7 +4774,9 @@
       <c r="I73" s="7"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B74" s="8"/>
+      <c r="B74" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
@@ -4772,9 +4786,7 @@
       <c r="I74" s="7"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B75" s="8" t="s">
-        <v>39</v>
-      </c>
+      <c r="B75" s="8"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
@@ -4785,7 +4797,7 @@
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
@@ -4797,7 +4809,7 @@
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
@@ -4808,7 +4820,9 @@
       <c r="I77" s="7"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B78" s="8"/>
+      <c r="B78" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
@@ -4818,9 +4832,7 @@
       <c r="I78" s="7"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B79" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="B79" s="8"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
@@ -4830,7 +4842,9 @@
       <c r="I79" s="7"/>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B80" s="8"/>
+      <c r="B80" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
@@ -4840,9 +4854,7 @@
       <c r="I80" s="7"/>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B81" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="B81" s="8"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
@@ -4850,16 +4862,11 @@
       <c r="G81" s="6"/>
       <c r="H81" s="6"/>
       <c r="I81" s="7"/>
-      <c r="J81" t="str">
-        <f>$J$68</f>
-        <v>→</v>
-      </c>
-      <c r="K81" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B82" s="8"/>
+      <c r="B82" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
@@ -4867,11 +4874,16 @@
       <c r="G82" s="6"/>
       <c r="H82" s="6"/>
       <c r="I82" s="7"/>
+      <c r="J82" t="str">
+        <f>$J$69</f>
+        <v>→</v>
+      </c>
+      <c r="K82" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B83" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="B83" s="8"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
@@ -4881,7 +4893,9 @@
       <c r="I83" s="7"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B84" s="8"/>
+      <c r="B84" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
@@ -4891,9 +4905,7 @@
       <c r="I84" s="7"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B85" s="8" t="s">
-        <v>45</v>
-      </c>
+      <c r="B85" s="8"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
@@ -4903,7 +4915,9 @@
       <c r="I85" s="7"/>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B86" s="8"/>
+      <c r="B86" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
@@ -4913,9 +4927,7 @@
       <c r="I86" s="7"/>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B87" s="8" t="s">
-        <v>46</v>
-      </c>
+      <c r="B87" s="8"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
       <c r="E87" s="6"/>
@@ -4925,7 +4937,9 @@
       <c r="I87" s="7"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B88" s="8"/>
+      <c r="B88" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
       <c r="E88" s="6"/>
@@ -4935,9 +4949,7 @@
       <c r="I88" s="7"/>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B89" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="B89" s="8"/>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
@@ -4948,7 +4960,7 @@
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
@@ -4957,15 +4969,11 @@
       <c r="G90" s="6"/>
       <c r="H90" s="6"/>
       <c r="I90" s="7"/>
-      <c r="J90" t="s">
-        <v>17</v>
-      </c>
-      <c r="K90" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B91" s="8"/>
+      <c r="B91" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
@@ -4973,11 +4981,15 @@
       <c r="G91" s="6"/>
       <c r="H91" s="6"/>
       <c r="I91" s="7"/>
+      <c r="J91" t="s">
+        <v>17</v>
+      </c>
+      <c r="K91" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B92" s="8" t="s">
-        <v>49</v>
-      </c>
+      <c r="B92" s="8"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
@@ -4988,7 +5000,7 @@
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B93" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
@@ -4999,7 +5011,9 @@
       <c r="I93" s="7"/>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B94" s="8"/>
+      <c r="B94" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
@@ -5009,9 +5023,7 @@
       <c r="I94" s="7"/>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B95" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="B95" s="8"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
       <c r="E95" s="6"/>
@@ -5021,7 +5033,9 @@
       <c r="I95" s="7"/>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B96" s="8"/>
+      <c r="B96" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
       <c r="E96" s="6"/>
@@ -5031,53 +5045,48 @@
       <c r="I96" s="7"/>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B97" s="9" t="s">
+      <c r="B97" s="8"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="7"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B98" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="10"/>
-      <c r="F97" s="10"/>
-      <c r="G97" s="10"/>
-      <c r="H97" s="10"/>
-      <c r="I97" s="11"/>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="11"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B101" s="2" t="s">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B102" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
-      <c r="J101" s="3"/>
-      <c r="K101" s="3"/>
-      <c r="L101" s="3"/>
-      <c r="M101" s="3"/>
-      <c r="N101" s="4"/>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B102" s="8"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="6"/>
-      <c r="F102" s="6"/>
-      <c r="G102" s="6"/>
-      <c r="H102" s="6"/>
-      <c r="I102" s="6"/>
-      <c r="J102" s="6"/>
-      <c r="K102" s="6"/>
-      <c r="L102" s="6"/>
-      <c r="M102" s="6"/>
-      <c r="N102" s="7"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+      <c r="M102" s="3"/>
+      <c r="N102" s="4"/>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B103" s="8"/>
@@ -5365,19 +5374,34 @@
       <c r="N121" s="7"/>
     </row>
     <row r="122" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B122" s="9"/>
-      <c r="C122" s="10"/>
-      <c r="D122" s="10"/>
-      <c r="E122" s="10"/>
-      <c r="F122" s="10"/>
-      <c r="G122" s="10"/>
-      <c r="H122" s="10"/>
-      <c r="I122" s="10"/>
-      <c r="J122" s="10"/>
-      <c r="K122" s="10"/>
-      <c r="L122" s="10"/>
-      <c r="M122" s="10"/>
-      <c r="N122" s="11"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="6"/>
+      <c r="I122" s="6"/>
+      <c r="J122" s="6"/>
+      <c r="K122" s="6"/>
+      <c r="L122" s="6"/>
+      <c r="M122" s="6"/>
+      <c r="N122" s="7"/>
+    </row>
+    <row r="123" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B123" s="9"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
+      <c r="G123" s="10"/>
+      <c r="H123" s="10"/>
+      <c r="I123" s="10"/>
+      <c r="J123" s="10"/>
+      <c r="K123" s="10"/>
+      <c r="L123" s="10"/>
+      <c r="M123" s="10"/>
+      <c r="N123" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>